<commit_message>
Add OMB Approval Date to Survey if OMB Approval code entered
</commit_message>
<xml_diff>
--- a/test/fixtures/files/TestGenericTemplateMini.xlsx
+++ b/test/fixtures/files/TestGenericTemplateMini.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghamilton/devel/CDC/SDPV/SDP-Vocabulary-Service/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEB9B41-EB24-D24F-8CFE-ABA23A90F369}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39E3E02-AAE9-8F44-A6F2-EC7FE63F9AC6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="929" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="8" r:id="rId1"/>
@@ -737,9 +737,6 @@
     <t>END: Cell Phone County</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>Response Set Name (R)</t>
   </si>
   <si>
@@ -759,6 +756,9 @@
   </si>
   <si>
     <t>This is the Yes No DK Refused Response</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -1341,10 +1341,10 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1438,10 +1438,10 @@
         <v>228</v>
       </c>
       <c r="B5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>229</v>
@@ -1587,19 +1587,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1703,19 +1703,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1839,19 +1839,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1995,19 +1995,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2295,19 +2295,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2682,8 +2682,8 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2697,19 +2697,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2717,7 +2717,7 @@
         <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>63</v>
@@ -2780,19 +2780,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>